<commit_message>
fix page issue with the jvm14 table, add some diagrams and developer notes on the implementation
</commit_message>
<xml_diff>
--- a/jvm14.xlsx
+++ b/jvm14.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\school\Diplomarbeit\documents\sources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\school\Diplomarbeit\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C615EB-D40C-46C4-9E80-88F55AB2971D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0080ECE4-DF78-4489-BDDC-FA4909AFCE3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{A4882BE5-527C-4E5D-8971-46616601A2BB}"/>
   </bookViews>
@@ -2814,42 +2814,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2861,12 +2825,48 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent2" xfId="1" builtinId="33"/>
@@ -3185,7 +3185,7 @@
   <dimension ref="A1:F123"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F115" sqref="F115"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3199,167 +3199,167 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="40" t="s">
         <v>217</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="74"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="42"/>
     </row>
     <row r="2" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="48" t="s">
         <v>220</v>
       </c>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="43" t="s">
         <v>230</v>
       </c>
-      <c r="C2" s="76"/>
+      <c r="C2" s="44"/>
       <c r="D2" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="53" t="s">
         <v>231</v>
       </c>
-      <c r="F2" s="51"/>
+      <c r="F2" s="54"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="71"/>
-      <c r="B3" s="61" t="s">
+      <c r="A3" s="50"/>
+      <c r="B3" s="45" t="s">
         <v>218</v>
       </c>
-      <c r="C3" s="63"/>
+      <c r="C3" s="46"/>
       <c r="D3" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="55" t="s">
         <v>232</v>
       </c>
-      <c r="F3" s="47"/>
+      <c r="F3" s="56"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="71"/>
-      <c r="B4" s="61" t="s">
+      <c r="A4" s="50"/>
+      <c r="B4" s="45" t="s">
         <v>219</v>
       </c>
-      <c r="C4" s="63"/>
+      <c r="C4" s="46"/>
       <c r="D4" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="55" t="s">
         <v>233</v>
       </c>
-      <c r="F4" s="47"/>
+      <c r="F4" s="56"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="71"/>
-      <c r="B5" s="55" t="s">
+      <c r="A5" s="50"/>
+      <c r="B5" s="51" t="s">
         <v>221</v>
       </c>
-      <c r="C5" s="57"/>
+      <c r="C5" s="52"/>
       <c r="D5" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="E5" s="40" t="s">
+      <c r="E5" s="57" t="s">
         <v>234</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="58"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="15"/>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="51" t="s">
         <v>226</v>
       </c>
-      <c r="C6" s="57"/>
+      <c r="C6" s="52"/>
       <c r="D6" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="E6" s="40" t="s">
+      <c r="E6" s="57" t="s">
         <v>235</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="58"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="51" t="s">
         <v>228</v>
       </c>
-      <c r="C7" s="57"/>
+      <c r="C7" s="52"/>
       <c r="D7" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="57" t="s">
         <v>236</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="58"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="17"/>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="51" t="s">
         <v>225</v>
       </c>
-      <c r="C8" s="57"/>
+      <c r="C8" s="52"/>
       <c r="D8" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="57" t="s">
         <v>237</v>
       </c>
-      <c r="F8" s="41"/>
-    </row>
-    <row r="9" spans="1:6" ht="3.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="58"/>
+    </row>
+    <row r="9" spans="1:6" ht="2.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="64" t="s">
+      <c r="A10" s="59" t="s">
         <v>243</v>
       </c>
-      <c r="B10" s="65"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="66"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="61"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="44" t="s">
+      <c r="B11" s="62"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="62" t="s">
         <v>238</v>
       </c>
-      <c r="E11" s="44"/>
-      <c r="F11" s="51"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="54"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="55" t="s">
         <v>239</v>
       </c>
-      <c r="B12" s="46"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="46" t="s">
+      <c r="B12" s="63"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="63" t="s">
         <v>290</v>
       </c>
-      <c r="E12" s="46"/>
-      <c r="F12" s="47"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="56"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="55" t="s">
         <v>240</v>
       </c>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="61" t="s">
+      <c r="B13" s="63"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="45" t="s">
         <v>241</v>
       </c>
-      <c r="E13" s="62"/>
-      <c r="F13" s="63"/>
-    </row>
-    <row r="14" spans="1:6" ht="3.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="64"/>
+      <c r="F13" s="46"/>
+    </row>
+    <row r="14" spans="1:6" ht="2.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="D14" s="3"/>
@@ -3367,14 +3367,14 @@
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="64" t="s">
+      <c r="A15" s="59" t="s">
         <v>242</v>
       </c>
-      <c r="B15" s="65"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="66"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="61"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="67" t="s">
@@ -3382,49 +3382,49 @@
       </c>
       <c r="B16" s="68"/>
       <c r="C16" s="69"/>
-      <c r="D16" s="59" t="s">
+      <c r="D16" s="65" t="s">
         <v>286</v>
       </c>
-      <c r="E16" s="59"/>
-      <c r="F16" s="60"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="66"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="52" t="s">
+      <c r="A17" s="73" t="s">
         <v>245</v>
       </c>
-      <c r="B17" s="53"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="55" t="s">
+      <c r="B17" s="74"/>
+      <c r="C17" s="75"/>
+      <c r="D17" s="51" t="s">
         <v>287</v>
       </c>
-      <c r="E17" s="56"/>
-      <c r="F17" s="57"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="52"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="52" t="s">
+      <c r="A18" s="73" t="s">
         <v>246</v>
       </c>
-      <c r="B18" s="53"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="58" t="s">
+      <c r="B18" s="74"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="78" t="s">
         <v>288</v>
       </c>
-      <c r="E18" s="59"/>
-      <c r="F18" s="60"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="66"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="57" t="s">
         <v>247</v>
       </c>
-      <c r="B19" s="42"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="55" t="s">
+      <c r="B19" s="76"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="51" t="s">
         <v>289</v>
       </c>
-      <c r="E19" s="56"/>
-      <c r="F19" s="57"/>
-    </row>
-    <row r="20" spans="1:6" ht="3.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="77"/>
+      <c r="F19" s="52"/>
+    </row>
+    <row r="20" spans="1:6" ht="2.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="11"/>
@@ -3433,224 +3433,224 @@
       <c r="F20" s="7"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="48" t="s">
+      <c r="A21" s="70" t="s">
         <v>248</v>
       </c>
-      <c r="B21" s="49"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="50"/>
+      <c r="B21" s="71"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="72"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="53" t="s">
         <v>249</v>
       </c>
-      <c r="B22" s="44"/>
-      <c r="C22" s="44"/>
+      <c r="B22" s="62"/>
+      <c r="C22" s="62"/>
       <c r="D22" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="E22" s="43" t="s">
+      <c r="E22" s="53" t="s">
         <v>270</v>
       </c>
-      <c r="F22" s="51"/>
+      <c r="F22" s="54"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="55" t="s">
         <v>249</v>
       </c>
-      <c r="B23" s="46"/>
-      <c r="C23" s="47"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="56"/>
       <c r="D23" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="E23" s="45" t="s">
+      <c r="E23" s="55" t="s">
         <v>271</v>
       </c>
-      <c r="F23" s="47"/>
+      <c r="F23" s="56"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="45" t="s">
+      <c r="A24" s="55" t="s">
         <v>250</v>
       </c>
-      <c r="B24" s="46"/>
-      <c r="C24" s="47"/>
+      <c r="B24" s="63"/>
+      <c r="C24" s="56"/>
       <c r="D24" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="E24" s="45" t="s">
+      <c r="E24" s="55" t="s">
         <v>272</v>
       </c>
-      <c r="F24" s="47"/>
+      <c r="F24" s="56"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="40" t="s">
+      <c r="A25" s="57" t="s">
         <v>251</v>
       </c>
-      <c r="B25" s="42"/>
-      <c r="C25" s="41"/>
+      <c r="B25" s="76"/>
+      <c r="C25" s="58"/>
       <c r="D25" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="E25" s="40" t="s">
+      <c r="E25" s="57" t="s">
         <v>273</v>
       </c>
-      <c r="F25" s="41"/>
+      <c r="F25" s="58"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="40" t="s">
+      <c r="A26" s="57" t="s">
         <v>250</v>
       </c>
-      <c r="B26" s="42"/>
-      <c r="C26" s="41"/>
+      <c r="B26" s="76"/>
+      <c r="C26" s="58"/>
       <c r="D26" s="13" t="s">
         <v>259</v>
       </c>
-      <c r="E26" s="40" t="s">
+      <c r="E26" s="57" t="s">
         <v>274</v>
       </c>
-      <c r="F26" s="41"/>
+      <c r="F26" s="58"/>
     </row>
     <row r="27" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="57" t="s">
         <v>250</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="41"/>
+      <c r="B27" s="76"/>
+      <c r="C27" s="58"/>
       <c r="D27" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="E27" s="40" t="s">
+      <c r="E27" s="57" t="s">
         <v>276</v>
       </c>
-      <c r="F27" s="41"/>
+      <c r="F27" s="58"/>
     </row>
     <row r="28" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="40" t="s">
+      <c r="A28" s="57" t="s">
         <v>250</v>
       </c>
-      <c r="B28" s="42"/>
-      <c r="C28" s="41"/>
+      <c r="B28" s="76"/>
+      <c r="C28" s="58"/>
       <c r="D28" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="E28" s="40" t="s">
+      <c r="E28" s="57" t="s">
         <v>277</v>
       </c>
-      <c r="F28" s="41"/>
+      <c r="F28" s="58"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="57" t="s">
         <v>250</v>
       </c>
-      <c r="B29" s="42"/>
-      <c r="C29" s="41"/>
+      <c r="B29" s="76"/>
+      <c r="C29" s="58"/>
       <c r="D29" s="13" t="s">
         <v>262</v>
       </c>
-      <c r="E29" s="40" t="s">
+      <c r="E29" s="57" t="s">
         <v>280</v>
       </c>
-      <c r="F29" s="41"/>
+      <c r="F29" s="58"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="57" t="s">
         <v>250</v>
       </c>
-      <c r="B30" s="42"/>
-      <c r="C30" s="41"/>
+      <c r="B30" s="76"/>
+      <c r="C30" s="58"/>
       <c r="D30" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="E30" s="40" t="s">
+      <c r="E30" s="57" t="s">
         <v>283</v>
       </c>
-      <c r="F30" s="41"/>
+      <c r="F30" s="58"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="57" t="s">
         <v>250</v>
       </c>
-      <c r="B31" s="42"/>
-      <c r="C31" s="41"/>
+      <c r="B31" s="76"/>
+      <c r="C31" s="58"/>
       <c r="D31" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="E31" s="40" t="s">
+      <c r="E31" s="57" t="s">
         <v>279</v>
       </c>
-      <c r="F31" s="41"/>
+      <c r="F31" s="58"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="57" t="s">
         <v>252</v>
       </c>
-      <c r="B32" s="42"/>
-      <c r="C32" s="41"/>
+      <c r="B32" s="76"/>
+      <c r="C32" s="58"/>
       <c r="D32" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="E32" s="40" t="s">
+      <c r="E32" s="57" t="s">
         <v>282</v>
       </c>
-      <c r="F32" s="41"/>
+      <c r="F32" s="58"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="40" t="s">
+      <c r="A33" s="57" t="s">
         <v>250</v>
       </c>
-      <c r="B33" s="42"/>
-      <c r="C33" s="41"/>
+      <c r="B33" s="76"/>
+      <c r="C33" s="58"/>
       <c r="D33" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="E33" s="40" t="s">
+      <c r="E33" s="57" t="s">
         <v>278</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="58"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="40" t="s">
+      <c r="A34" s="57" t="s">
         <v>253</v>
       </c>
-      <c r="B34" s="42"/>
-      <c r="C34" s="41"/>
+      <c r="B34" s="76"/>
+      <c r="C34" s="58"/>
       <c r="D34" s="13" t="s">
         <v>267</v>
       </c>
-      <c r="E34" s="40" t="s">
+      <c r="E34" s="57" t="s">
         <v>281</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="58"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="40" t="s">
+      <c r="A35" s="57" t="s">
         <v>250</v>
       </c>
-      <c r="B35" s="42"/>
-      <c r="C35" s="41"/>
+      <c r="B35" s="76"/>
+      <c r="C35" s="58"/>
       <c r="D35" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="E35" s="40" t="s">
+      <c r="E35" s="57" t="s">
         <v>284</v>
       </c>
-      <c r="F35" s="41"/>
+      <c r="F35" s="58"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="40" t="s">
+      <c r="A36" s="57" t="s">
         <v>254</v>
       </c>
-      <c r="B36" s="42"/>
-      <c r="C36" s="41"/>
+      <c r="B36" s="76"/>
+      <c r="C36" s="58"/>
       <c r="D36" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="E36" s="40" t="s">
+      <c r="E36" s="57" t="s">
         <v>285</v>
       </c>
-      <c r="F36" s="41"/>
+      <c r="F36" s="58"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="8"/>
@@ -3671,7 +3671,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="70" t="s">
+      <c r="A38" s="48" t="s">
         <v>119</v>
       </c>
       <c r="B38" s="26" t="s">
@@ -3691,7 +3691,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="70"/>
+      <c r="A39" s="48"/>
       <c r="B39" s="20" t="s">
         <v>6</v>
       </c>
@@ -3709,7 +3709,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="70"/>
+      <c r="A40" s="48"/>
       <c r="B40" s="20" t="s">
         <v>7</v>
       </c>
@@ -3727,7 +3727,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="70"/>
+      <c r="A41" s="48"/>
       <c r="B41" s="20" t="s">
         <v>8</v>
       </c>
@@ -3745,7 +3745,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="70"/>
+      <c r="A42" s="48"/>
       <c r="B42" s="20" t="s">
         <v>9</v>
       </c>
@@ -3763,7 +3763,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="70"/>
+      <c r="A43" s="48"/>
       <c r="B43" s="20" t="s">
         <v>10</v>
       </c>
@@ -3781,7 +3781,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="70"/>
+      <c r="A44" s="48"/>
       <c r="B44" s="20" t="s">
         <v>11</v>
       </c>
@@ -3799,7 +3799,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="70"/>
+      <c r="A45" s="48"/>
       <c r="B45" s="20" t="s">
         <v>12</v>
       </c>
@@ -3817,7 +3817,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="70"/>
+      <c r="A46" s="48"/>
       <c r="B46" s="20" t="s">
         <v>30</v>
       </c>
@@ -3835,7 +3835,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="70"/>
+      <c r="A47" s="48"/>
       <c r="B47" s="20" t="s">
         <v>31</v>
       </c>
@@ -3853,7 +3853,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="78"/>
+      <c r="A48" s="49"/>
       <c r="B48" s="24" t="s">
         <v>32</v>
       </c>
@@ -3871,7 +3871,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="71" t="s">
+      <c r="A49" s="50" t="s">
         <v>121</v>
       </c>
       <c r="B49" s="28" t="s">
@@ -3891,7 +3891,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="71"/>
+      <c r="A50" s="50"/>
       <c r="B50" s="20" t="s">
         <v>33</v>
       </c>
@@ -3909,7 +3909,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="71"/>
+      <c r="A51" s="50"/>
       <c r="B51" s="20" t="s">
         <v>34</v>
       </c>
@@ -3927,7 +3927,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="71"/>
+      <c r="A52" s="50"/>
       <c r="B52" s="20" t="s">
         <v>35</v>
       </c>
@@ -3945,7 +3945,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="71"/>
+      <c r="A53" s="50"/>
       <c r="B53" s="20" t="s">
         <v>36</v>
       </c>
@@ -3963,7 +3963,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="71"/>
+      <c r="A54" s="50"/>
       <c r="B54" s="20" t="s">
         <v>37</v>
       </c>
@@ -3981,7 +3981,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="71"/>
+      <c r="A55" s="50"/>
       <c r="B55" s="20" t="s">
         <v>193</v>
       </c>
@@ -3999,7 +3999,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="71"/>
+      <c r="A56" s="50"/>
       <c r="B56" s="20" t="s">
         <v>38</v>
       </c>
@@ -4017,7 +4017,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="71"/>
+      <c r="A57" s="50"/>
       <c r="B57" s="20" t="s">
         <v>39</v>
       </c>
@@ -4035,7 +4035,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="71"/>
+      <c r="A58" s="50"/>
       <c r="B58" s="20" t="s">
         <v>40</v>
       </c>
@@ -4053,7 +4053,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="71"/>
+      <c r="A59" s="50"/>
       <c r="B59" s="20" t="s">
         <v>41</v>
       </c>
@@ -4071,7 +4071,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="71"/>
+      <c r="A60" s="50"/>
       <c r="B60" s="20" t="s">
         <v>202</v>
       </c>
@@ -4089,7 +4089,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="71"/>
+      <c r="A61" s="50"/>
       <c r="B61" s="33" t="s">
         <v>200</v>
       </c>
@@ -4107,7 +4107,7 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="77" t="s">
+      <c r="A62" s="47" t="s">
         <v>275</v>
       </c>
       <c r="B62" s="24" t="s">
@@ -4127,7 +4127,7 @@
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="70"/>
+      <c r="A63" s="48"/>
       <c r="B63" s="28" t="s">
         <v>43</v>
       </c>
@@ -4145,7 +4145,7 @@
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="70"/>
+      <c r="A64" s="48"/>
       <c r="B64" s="24" t="s">
         <v>44</v>
       </c>
@@ -4163,7 +4163,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="70"/>
+      <c r="A65" s="48"/>
       <c r="B65" s="24" t="s">
         <v>45</v>
       </c>
@@ -4181,7 +4181,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="70"/>
+      <c r="A66" s="48"/>
       <c r="B66" s="24" t="s">
         <v>46</v>
       </c>
@@ -4199,7 +4199,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="70"/>
+      <c r="A67" s="48"/>
       <c r="B67" s="24" t="s">
         <v>47</v>
       </c>
@@ -4217,7 +4217,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="70"/>
+      <c r="A68" s="48"/>
       <c r="B68" s="27" t="s">
         <v>48</v>
       </c>
@@ -4235,7 +4235,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="70"/>
+      <c r="A69" s="48"/>
       <c r="B69" s="27" t="s">
         <v>49</v>
       </c>
@@ -4253,7 +4253,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="70"/>
+      <c r="A70" s="48"/>
       <c r="B70" s="24" t="s">
         <v>50</v>
       </c>
@@ -4271,7 +4271,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="70"/>
+      <c r="A71" s="48"/>
       <c r="B71" s="24" t="s">
         <v>51</v>
       </c>
@@ -4289,7 +4289,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="70"/>
+      <c r="A72" s="48"/>
       <c r="B72" s="24" t="s">
         <v>52</v>
       </c>
@@ -4307,7 +4307,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="70"/>
+      <c r="A73" s="48"/>
       <c r="B73" s="24" t="s">
         <v>205</v>
       </c>
@@ -4325,7 +4325,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="78"/>
+      <c r="A74" s="49"/>
       <c r="B74" s="24" t="s">
         <v>207</v>
       </c>
@@ -4343,7 +4343,7 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="70" t="s">
+      <c r="A75" s="48" t="s">
         <v>4</v>
       </c>
       <c r="B75" s="35" t="s">
@@ -4363,7 +4363,7 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="70"/>
+      <c r="A76" s="48"/>
       <c r="B76" s="35" t="s">
         <v>75</v>
       </c>
@@ -4381,7 +4381,7 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="78"/>
+      <c r="A77" s="49"/>
       <c r="B77" s="35" t="s">
         <v>76</v>
       </c>
@@ -4399,7 +4399,7 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="77" t="s">
+      <c r="A78" s="47" t="s">
         <v>120</v>
       </c>
       <c r="B78" s="34" t="s">
@@ -4419,7 +4419,7 @@
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="70"/>
+      <c r="A79" s="48"/>
       <c r="B79" s="34" t="s">
         <v>63</v>
       </c>
@@ -4437,7 +4437,7 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="70"/>
+      <c r="A80" s="48"/>
       <c r="B80" s="34" t="s">
         <v>64</v>
       </c>
@@ -4455,7 +4455,7 @@
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="70"/>
+      <c r="A81" s="48"/>
       <c r="B81" s="34" t="s">
         <v>65</v>
       </c>
@@ -4473,7 +4473,7 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="70"/>
+      <c r="A82" s="48"/>
       <c r="B82" s="34" t="s">
         <v>66</v>
       </c>
@@ -4491,7 +4491,7 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83" s="70"/>
+      <c r="A83" s="48"/>
       <c r="B83" s="34" t="s">
         <v>67</v>
       </c>
@@ -4509,7 +4509,7 @@
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" s="70"/>
+      <c r="A84" s="48"/>
       <c r="B84" s="34" t="s">
         <v>68</v>
       </c>
@@ -4527,7 +4527,7 @@
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="70"/>
+      <c r="A85" s="48"/>
       <c r="B85" s="34" t="s">
         <v>69</v>
       </c>
@@ -4545,7 +4545,7 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86" s="78"/>
+      <c r="A86" s="49"/>
       <c r="B86" s="34" t="s">
         <v>70</v>
       </c>
@@ -4563,7 +4563,7 @@
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A87" s="70" t="s">
+      <c r="A87" s="48" t="s">
         <v>145</v>
       </c>
       <c r="B87" s="34" t="s">
@@ -4583,7 +4583,7 @@
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" s="70"/>
+      <c r="A88" s="48"/>
       <c r="B88" s="34" t="s">
         <v>79</v>
       </c>
@@ -4601,7 +4601,7 @@
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89" s="70"/>
+      <c r="A89" s="48"/>
       <c r="B89" s="34" t="s">
         <v>80</v>
       </c>
@@ -4619,7 +4619,7 @@
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A90" s="70"/>
+      <c r="A90" s="48"/>
       <c r="B90" s="34" t="s">
         <v>81</v>
       </c>
@@ -4637,7 +4637,7 @@
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A91" s="70"/>
+      <c r="A91" s="48"/>
       <c r="B91" s="34" t="s">
         <v>82</v>
       </c>
@@ -4655,7 +4655,7 @@
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A92" s="70"/>
+      <c r="A92" s="48"/>
       <c r="B92" s="34" t="s">
         <v>83</v>
       </c>
@@ -4673,7 +4673,7 @@
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A93" s="70"/>
+      <c r="A93" s="48"/>
       <c r="B93" s="34" t="s">
         <v>84</v>
       </c>
@@ -4691,7 +4691,7 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A94" s="70"/>
+      <c r="A94" s="48"/>
       <c r="B94" s="34" t="s">
         <v>85</v>
       </c>
@@ -4709,7 +4709,7 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A95" s="70"/>
+      <c r="A95" s="48"/>
       <c r="B95" s="34" t="s">
         <v>86</v>
       </c>
@@ -4727,7 +4727,7 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A96" s="70"/>
+      <c r="A96" s="48"/>
       <c r="B96" s="34" t="s">
         <v>87</v>
       </c>
@@ -4745,7 +4745,7 @@
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A97" s="70"/>
+      <c r="A97" s="48"/>
       <c r="B97" s="34" t="s">
         <v>88</v>
       </c>
@@ -4763,7 +4763,7 @@
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98" s="70"/>
+      <c r="A98" s="48"/>
       <c r="B98" s="34" t="s">
         <v>89</v>
       </c>
@@ -4781,7 +4781,7 @@
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" s="70"/>
+      <c r="A99" s="48"/>
       <c r="B99" s="34" t="s">
         <v>92</v>
       </c>
@@ -4799,7 +4799,7 @@
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A100" s="78"/>
+      <c r="A100" s="49"/>
       <c r="B100" s="31" t="s">
         <v>90</v>
       </c>
@@ -4817,7 +4817,7 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A101" s="77" t="s">
+      <c r="A101" s="47" t="s">
         <v>122</v>
       </c>
       <c r="B101" s="34" t="s">
@@ -4837,7 +4837,7 @@
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A102" s="70"/>
+      <c r="A102" s="48"/>
       <c r="B102" s="34" t="s">
         <v>96</v>
       </c>
@@ -4855,7 +4855,7 @@
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A103" s="70"/>
+      <c r="A103" s="48"/>
       <c r="B103" s="34" t="s">
         <v>97</v>
       </c>
@@ -4873,7 +4873,7 @@
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A104" s="78"/>
+      <c r="A104" s="49"/>
       <c r="B104" s="34" t="s">
         <v>98</v>
       </c>
@@ -4891,7 +4891,7 @@
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A105" s="77" t="s">
+      <c r="A105" s="47" t="s">
         <v>123</v>
       </c>
       <c r="B105" s="31" t="s">
@@ -4911,7 +4911,7 @@
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A106" s="70"/>
+      <c r="A106" s="48"/>
       <c r="B106" s="31" t="s">
         <v>110</v>
       </c>
@@ -4929,7 +4929,7 @@
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A107" s="70"/>
+      <c r="A107" s="48"/>
       <c r="B107" s="34" t="s">
         <v>111</v>
       </c>
@@ -4947,7 +4947,7 @@
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A108" s="70"/>
+      <c r="A108" s="48"/>
       <c r="B108" s="34" t="s">
         <v>112</v>
       </c>
@@ -4965,7 +4965,7 @@
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A109" s="70"/>
+      <c r="A109" s="48"/>
       <c r="B109" s="39" t="s">
         <v>215</v>
       </c>
@@ -4983,7 +4983,7 @@
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A110" s="70"/>
+      <c r="A110" s="48"/>
       <c r="B110" s="39" t="s">
         <v>349</v>
       </c>
@@ -5001,7 +5001,7 @@
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A111" s="70"/>
+      <c r="A111" s="48"/>
       <c r="B111" s="34" t="s">
         <v>113</v>
       </c>
@@ -5019,7 +5019,7 @@
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A112" s="70"/>
+      <c r="A112" s="48"/>
       <c r="B112" s="34" t="s">
         <v>114</v>
       </c>
@@ -5037,7 +5037,7 @@
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A113" s="70"/>
+      <c r="A113" s="48"/>
       <c r="B113" s="31" t="s">
         <v>115</v>
       </c>
@@ -5055,7 +5055,7 @@
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A114" s="70"/>
+      <c r="A114" s="48"/>
       <c r="B114" s="34" t="s">
         <v>116</v>
       </c>
@@ -5073,7 +5073,7 @@
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A115" s="70"/>
+      <c r="A115" s="48"/>
       <c r="B115" s="34" t="s">
         <v>354</v>
       </c>
@@ -5091,7 +5091,7 @@
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A116" s="78"/>
+      <c r="A116" s="49"/>
       <c r="B116" s="34" t="s">
         <v>117</v>
       </c>
@@ -5166,6 +5166,61 @@
     </row>
   </sheetData>
   <mergeCells count="71">
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -5182,61 +5237,6 @@
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A36:C36"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>